<commit_message>
Added synchronisation of server's AIs
</commit_message>
<xml_diff>
--- a/Protocol plan.xlsx
+++ b/Protocol plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Create</t>
   </si>
@@ -30,9 +30,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>0 - Soldier</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>id, x, y</t>
   </si>
   <si>
-    <t>1 - Building</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -69,22 +63,37 @@
     <t>Temple</t>
   </si>
   <si>
-    <t>0/1,x,y</t>
-  </si>
-  <si>
-    <t>First parametre is create/destroy</t>
-  </si>
-  <si>
-    <t>x,y, [id]</t>
-  </si>
-  <si>
-    <t>id only sent by server</t>
-  </si>
-  <si>
-    <t>2 - Country update</t>
-  </si>
-  <si>
-    <t>Done by server as well</t>
+    <t>Die</t>
+  </si>
+  <si>
+    <t>Country number</t>
+  </si>
+  <si>
+    <t>10 - Soldier</t>
+  </si>
+  <si>
+    <t>11 - Building</t>
+  </si>
+  <si>
+    <t>12 - Country update</t>
+  </si>
+  <si>
+    <t>13 - Country</t>
+  </si>
+  <si>
+    <t>Done by server only</t>
+  </si>
+  <si>
+    <t>x,y[, id, country]</t>
+  </si>
+  <si>
+    <t>id &amp; country only sent by server</t>
+  </si>
+  <si>
+    <t>0/1,x,y[, country]</t>
+  </si>
+  <si>
+    <t>First parametre is destroy/create</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -190,49 +199,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -315,11 +285,100 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -330,7 +389,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -340,45 +401,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -387,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -423,11 +449,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -442,26 +467,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,16 +797,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
@@ -782,27 +814,31 @@
     <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>5</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="12">
         <v>0</v>
@@ -813,22 +849,26 @@
       <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="22">
         <v>0</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="22">
         <v>1</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="22">
         <v>2</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>7</v>
+      <c r="H2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="30">
+        <v>0</v>
+      </c>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -840,93 +880,105 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>8</v>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -936,7 +988,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -946,7 +998,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -956,7 +1008,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -966,7 +1018,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -976,7 +1028,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>

</xml_diff>

<commit_message>
Added in synchronisation for units.
</commit_message>
<xml_diff>
--- a/Protocol plan.xlsx
+++ b/Protocol plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Create</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Returns</t>
   </si>
   <si>
-    <t>id, x, y</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Die</t>
   </si>
   <si>
-    <t>Country number</t>
-  </si>
-  <si>
     <t>10 - Soldier</t>
   </si>
   <si>
@@ -94,6 +88,18 @@
   </si>
   <si>
     <t>First parametre is destroy/create</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x, y, id</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>country, money</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -285,43 +291,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -398,13 +367,57 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -413,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -467,33 +480,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -800,7 +816,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,29 +828,30 @@
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="21.140625" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="24"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -849,22 +866,24 @@
       <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="20">
         <v>0</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="20">
         <v>1</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="20">
         <v>2</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="30">
+      <c r="H2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="27">
         <v>0</v>
       </c>
-      <c r="J2" s="24"/>
+      <c r="J2" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -880,103 +899,111 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="24"/>
+        <v>19</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Doesn't work. Give up hope.
</commit_message>
<xml_diff>
--- a/Protocol plan.xlsx
+++ b/Protocol plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Create</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Done by server only</t>
   </si>
   <si>
-    <t>x,y[, id, country]</t>
-  </si>
-  <si>
     <t>id &amp; country only sent by server</t>
   </si>
   <si>
@@ -100,6 +97,18 @@
   </si>
   <si>
     <t>country, money</t>
+  </si>
+  <si>
+    <t>x,y[, id, country][, reserve]</t>
+  </si>
+  <si>
+    <t>14 - Diplomacy</t>
+  </si>
+  <si>
+    <t>Peace</t>
+  </si>
+  <si>
+    <t>War</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -381,19 +390,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -420,13 +416,46 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -502,14 +531,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -813,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,10 +868,10 @@
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="21.140625" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="10" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
@@ -851,9 +891,15 @@
       <c r="I1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="29"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="32"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -881,11 +927,19 @@
       <c r="I2" s="27">
         <v>0</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="29">
         <v>1</v>
       </c>
+      <c r="K2" s="27">
+        <v>0</v>
+      </c>
+      <c r="L2" s="33">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -913,39 +967,51 @@
       <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="31" t="s">
-        <v>26</v>
-      </c>
+      <c r="J3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>27</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
@@ -973,16 +1039,20 @@
       <c r="I5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="31" t="s">
-        <v>10</v>
-      </c>
+      <c r="J5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>10</v>
@@ -992,7 +1062,7 @@
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="18" t="s">
@@ -1001,11 +1071,15 @@
       <c r="I6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="32" t="s">
-        <v>10</v>
-      </c>
+      <c r="J6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1015,7 +1089,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1025,7 +1099,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1035,7 +1109,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1045,7 +1119,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1055,7 +1129,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1067,6 +1141,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added diplomacy protocol, corrected country death protocol.
</commit_message>
<xml_diff>
--- a/Protocol plan.xlsx
+++ b/Protocol plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Create</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>War</t>
+  </si>
+  <si>
+    <t>country, country</t>
   </si>
 </sst>
 </file>
@@ -856,7 +859,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +872,7 @@
     <col min="8" max="8" width="21.140625" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
     <col min="10" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1006,8 +1010,12 @@
       <c r="J4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="34"/>
+      <c r="K4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
@@ -1042,8 +1050,12 @@
       <c r="J5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="34"/>
+      <c r="K5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>10</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
@@ -1074,8 +1086,12 @@
       <c r="J6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>

</xml_diff>

<commit_message>
Cleaned up protocol plan and logs.
</commit_message>
<xml_diff>
--- a/Protocol plan.xlsx
+++ b/Protocol plan.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1159,28 +1157,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>